<commit_message>
Removed the need of LocationId
</commit_message>
<xml_diff>
--- a/Templates/BomTemplate.xlsx
+++ b/Templates/BomTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/690b8719eb6b5234/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\source\repos\HCarlb\FinancePriceCalculator\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{0EA00543-646D-4E8E-9C07-248CEB29E435}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2C05B27E-E411-432F-A2DE-1244A7C3194E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1F0718-3304-4B30-9460-4C552F679C94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{73BE4DE6-480C-4F97-A8D1-6A93424FA456}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
-  <si>
-    <t>ns2:Sender</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>ns4:Base</t>
   </si>
@@ -51,9 +48,6 @@
   </si>
   <si>
     <t>ns3:Quantity</t>
-  </si>
-  <si>
-    <t>ABC</t>
   </si>
   <si>
     <t>ABC123</t>
@@ -423,22 +417,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0242C6-14E7-48A7-9D71-87E231317C38}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,58 +447,46 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4">
         <v>33.33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added example. Changed prices
</commit_message>
<xml_diff>
--- a/Templates/BomTemplate.xlsx
+++ b/Templates/BomTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\source\repos\HCarlb\FinancePriceCalculator\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1F0718-3304-4B30-9460-4C552F679C94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975C55AD-EDC7-41B1-9DCF-D6DEDBA8E70D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{73BE4DE6-480C-4F97-A8D1-6A93424FA456}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="33960" windowHeight="15380" xr2:uid="{73BE4DE6-480C-4F97-A8D1-6A93424FA456}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>ns4:Base</t>
   </si>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0242C6-14E7-48A7-9D71-87E231317C38}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -456,7 +456,7 @@
         <v>6</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -464,13 +464,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -478,16 +475,33 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
       </c>
       <c r="E4">
-        <v>33.33</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>